<commit_message>
uc07 - revisão - WIP
</commit_message>
<xml_diff>
--- a/Documentação/Sprint 3/UC07_Registar_Freelancer/UC07_Registar_Freelancer_Plano_de_Testes.xlsx
+++ b/Documentação/Sprint 3/UC07_Registar_Freelancer/UC07_Registar_Freelancer_Plano_de_Testes.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="marta"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blest\Desktop\Sprints\upskill_java1_labprg_grupo2\Documentação\Sprint 3\UC07_Registar_Freelancer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924B84F3-70DB-4F89-9539-AE282F87EF2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="23260" windowHeight="12580" tabRatio="993"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="20730" windowHeight="11160" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId4"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:revision xmlns:pm="smNativeData" day="1614245675" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
@@ -206,96 +211,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
-    <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;"/>
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;$&quot;_-;\-* #,##0\ &quot;$&quot;_-;_-* &quot;-&quot;\ &quot;$&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
-    <numFmt numFmtId="14" formatCode="M/D/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="175" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614245675" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="240" lang="default"/>
-            <pm:cs face="Times New Roman" sz="240" lang="default"/>
-            <pm:ea face="SimSun" sz="240" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614245675" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="200" lang="default"/>
-            <pm:cs face="Times New Roman" sz="200" lang="default"/>
-            <pm:ea face="SimSun" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="8"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614245675" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="160" lang="default"/>
-            <pm:cs face="Times New Roman" sz="240" lang="default"/>
-            <pm:ea face="SimSun" sz="240" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614245675" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="200" lang="default"/>
-            <pm:cs face="Times New Roman" sz="240" lang="default"/>
-            <pm:ea face="SimSun" sz="240" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614245675" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="220" lang="default"/>
-            <pm:cs face="Times New Roman" sz="220" lang="default"/>
-            <pm:ea face="SimSun" sz="220" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,44 +246,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1614245675" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1614245675" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614245675"/>
-        </ext>
-      </extLst>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -358,63 +270,28 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614245675">
-            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
-            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
-            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
-            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
-          </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614245675"/>
-        </ext>
-      </extLst>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1">
       <alignment vertical="center"/>
-      <protection locked="0" hidden="0"/>
+      <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="bottom"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="1" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -422,25 +299,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Excel Built-in Note" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Excel Built-in Note" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
     <ext uri="smNativeData">
       <pm:charStyles xmlns:pm="smNativeData" id="1614245675" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
@@ -459,10 +343,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="D5D5D5"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="494949"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="EEECE1"/>
@@ -709,323 +593,308 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.60"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.696721" customWidth="1"/>
-    <col min="2" max="2" width="39.180328" customWidth="1" style="2"/>
-    <col min="3" max="4" width="34.401639" customWidth="1"/>
-    <col min="5" max="5" width="36.098361" customWidth="1"/>
-    <col min="6" max="6" width="33.598361" customWidth="1"/>
-    <col min="7" max="255" width="10.901639" customWidth="1"/>
+    <col min="1" max="1" width="23.75" customWidth="1"/>
+    <col min="2" max="2" width="39.125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="34.375" customWidth="1"/>
+    <col min="5" max="5" width="36.125" customWidth="1"/>
+    <col min="6" max="6" width="33.625" customWidth="1"/>
+    <col min="7" max="255" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="9">
+        <v>44238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="444" customHeight="1">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="4" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="4" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614245675" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614245675" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614245675" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1614245675" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1614245675" Id="1" type="0" value="0"/>
-      </ext>
-    </extLst>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.51180599999999998"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1614245675" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">

</xml_diff>